<commit_message>
this added last report 29-01-25
</commit_message>
<xml_diff>
--- a/DD-Profit_ROI/Mangrove Dec-24 Profit and Loss.xlsx
+++ b/DD-Profit_ROI/Mangrove Dec-24 Profit and Loss.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ED35EB-82DE-4D65-8C2B-559F7A8BF97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D13C85-BA4F-4AD0-8D82-5994AFA92CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,12 +64,6 @@
     <t>SC (Sales to Retail) Secondary</t>
   </si>
   <si>
-    <t>Distributor GA &amp; SAF Commission June'24</t>
-  </si>
-  <si>
-    <t>Distributor Campaign Shera partner June'24</t>
-  </si>
-  <si>
     <t>Accelerate</t>
   </si>
   <si>
@@ -182,6 +176,12 @@
   </si>
   <si>
     <t>Total Other Expenses</t>
+  </si>
+  <si>
+    <t>Distributor GA &amp; SAF Commission Dec'24</t>
+  </si>
+  <si>
+    <t>Distributor Campaign Shera partner Dec'24</t>
   </si>
 </sst>
 </file>
@@ -1229,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,16 +1375,18 @@
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="C13" s="16">
+        <v>2475</v>
+      </c>
       <c r="F13" s="11"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1393,16 +1395,18 @@
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="C15" s="16">
+        <v>2736</v>
+      </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="16">
         <v>150</v>
@@ -1415,14 +1419,14 @@
     </row>
     <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="21">
         <v>0</v>
       </c>
       <c r="C17" s="21">
         <f>SUM(C11:C16)</f>
-        <v>33578.339999999997</v>
+        <v>38789.339999999997</v>
       </c>
       <c r="G17" s="19"/>
     </row>
@@ -1444,7 +1448,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="82" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" s="83"/>
       <c r="C21" s="83"/>
@@ -1476,27 +1480,27 @@
         <v>6</v>
       </c>
       <c r="B24" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="E24" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="F24" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="G24" s="27" t="s">
         <v>20</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -1510,7 +1514,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" s="29">
         <v>10000</v>
@@ -1526,7 +1530,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
@@ -1540,7 +1544,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="29">
         <v>13000</v>
@@ -1556,7 +1560,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -1570,7 +1574,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -1584,7 +1588,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
@@ -1598,7 +1602,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -1612,7 +1616,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
@@ -1626,7 +1630,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
@@ -1640,7 +1644,7 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35" s="32">
         <v>1000</v>
@@ -1656,7 +1660,7 @@
     </row>
     <row r="36" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B36" s="35"/>
       <c r="C36" s="35"/>
@@ -1681,7 +1685,7 @@
     </row>
     <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="85" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B39" s="86"/>
       <c r="D39" s="38"/>
@@ -1691,23 +1695,23 @@
     </row>
     <row r="40" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D40" s="37"/>
       <c r="G40" s="39"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B41" s="42">
         <v>15440</v>
       </c>
       <c r="C41" s="87" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D41" s="88"/>
       <c r="E41" s="89"/>
@@ -1719,7 +1723,7 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42" s="42">
         <v>8000</v>
@@ -1732,23 +1736,23 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D43" s="54"/>
       <c r="E43" s="55"/>
       <c r="F43" s="62">
         <f>C17-F41</f>
-        <v>-28884.660000000003</v>
+        <v>-23673.660000000003</v>
       </c>
       <c r="G43" s="63"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" s="42">
         <v>700</v>
@@ -1761,7 +1765,7 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B45" s="42">
         <v>3758</v>
@@ -1774,7 +1778,7 @@
     </row>
     <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A46" s="43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" s="44">
         <v>8890</v>
@@ -1784,7 +1788,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" s="47">
         <v>1675</v>
@@ -1793,7 +1797,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" s="47"/>
       <c r="E48" s="38"/>
@@ -1801,21 +1805,21 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B49" s="44"/>
       <c r="G49" s="19"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" s="47"/>
       <c r="G50" s="19"/>
     </row>
     <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" s="49">
         <f>SUM(B41:B50)</f>

</xml_diff>